<commit_message>
TC02 - Validate Invalid Email Error
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TC02" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -77,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@</t>
   </si>
 </sst>
 </file>
@@ -175,8 +179,8 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,4 +269,48 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC03 - Verify error Message for mandatory fields
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TC02" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TC03" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -81,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">test@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000@test.io</t>
   </si>
 </sst>
 </file>
@@ -278,8 +282,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,4 +317,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC04 - error Message For Incorrect Values
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TC02" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="TC03" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="TC04" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -85,6 +86,27 @@
   </si>
   <si>
     <t xml:space="preserve">00000@test.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@test.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC@#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEFGHIJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@#$%&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@#</t>
   </si>
 </sst>
 </file>
@@ -94,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -115,6 +137,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,8 +188,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -184,14 +217,14 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,7 +319,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -326,13 +359,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,4 +394,125 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="test@test.io"/>
+    <hyperlink ref="B3" r:id="rId2" display="test@test.io"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC05 - Search Product
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TC02" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="TC03" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="TC04" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="TC05" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -217,7 +218,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="A1:A2 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,7 +317,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -360,7 +361,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -403,8 +404,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="A1:A2 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,4 +516,41 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC06 - Buy Product
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="TC03" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="TC04" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="TC05" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="TC06" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -62,7 +63,7 @@
     <t xml:space="preserve">http://automationpractice.com/index.php</t>
   </si>
   <si>
-    <t xml:space="preserve">rtrtryry@test.io</t>
+    <t xml:space="preserve">test0000@test.io</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
@@ -108,6 +109,18 @@
   </si>
   <si>
     <t xml:space="preserve">@#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
   </si>
 </sst>
 </file>
@@ -189,8 +202,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,14 +235,14 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="A1:A2 K2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,7 +284,7 @@
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -317,10 +334,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -361,10 +378,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -405,14 +422,14 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="A1:A2 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.1"/>
   </cols>
   <sheetData>
@@ -449,7 +466,7 @@
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -478,7 +495,7 @@
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -525,11 +542,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
   </cols>
@@ -542,6 +559,68 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC07 - Add to Wishlist error
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="TC04" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="TC05" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="TC06" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="TC07" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -121,6 +122,12 @@
   </si>
   <si>
     <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errorMsg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You must be logged in to manage your wishlist.</t>
   </si>
 </sst>
 </file>
@@ -202,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +222,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,7 +249,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
@@ -337,7 +348,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -381,7 +392,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -425,7 +436,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -546,7 +557,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
   </cols>
@@ -579,48 +590,92 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>30</v>
+      <c r="B1" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>31</v>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC08 - Verify total
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data.xlsx
+++ b/src/main/java/resources/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="TC05" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="TC06" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="TC07" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="TC08" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t xml:space="preserve">baseUrl</t>
   </si>
@@ -128,6 +129,12 @@
   </si>
   <si>
     <t xml:space="preserve">You must be logged in to manage your wishlist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incressQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
   </si>
 </sst>
 </file>
@@ -591,7 +598,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -652,7 +659,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -687,4 +694,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.62"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>